<commit_message>
Comment all writer.save() or writer.close()
In newer versions of the packages (pandas), it is not needed anymore to do this I think because otherwise it gives errors if you run writer.save() for example.
</commit_message>
<xml_diff>
--- a/1Water_treatment_model_USEPA/PSDM/Example_TCE.xlsx
+++ b/1Water_treatment_model_USEPA/PSDM/Example_TCE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JBurkhar\OneDrive - Environmental Protection Agency (EPA)\Profile\Desktop\Git\PSDM\PSDM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathieu\PycharmProjects\Thesis-Activated-Carbon-Modelling\1Water_treatment_model_USEPA\PSDM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="183" documentId="8_{FC6C552E-3166-4C64-8BC2-E954C229B3E9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{41008640-FEA6-4E03-9782-ECE2DD9879EE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA1F490-3FE3-4546-BB5F-2E7CFC9FA6AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{317BF3F6-A68C-4964-9BC3-AEDC7E3058F4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{317BF3F6-A68C-4964-9BC3-AEDC7E3058F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Properties" sheetId="1" r:id="rId1"/>
@@ -274,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -282,15 +282,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -617,21 +614,21 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -639,7 +636,7 @@
         <v>131.38999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -647,7 +644,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -655,7 +652,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -663,19 +660,19 @@
         <v>1.53</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>1100</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>9830</v>
       </c>
     </row>
@@ -688,18 +685,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB297697-1B90-46DD-B82E-FCE20BA48421}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -707,7 +704,7 @@
         <v>5026.04</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -715,7 +712,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -723,7 +720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -731,7 +728,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -749,163 +746,163 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>5.1299999999999998E-2</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>0.64100000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>0.80300000000000005</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>0.62</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>2.7650000000000001</v>
       </c>
       <c r="C8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>20000</v>
       </c>
       <c r="C9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>566.96600000000001</v>
       </c>
       <c r="C10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>10</v>
       </c>
       <c r="C11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="B14" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -919,18 +916,18 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -944,7 +941,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -954,11 +951,11 @@
       <c r="C2">
         <v>50000</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -972,7 +969,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -986,7 +983,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1010,18 +1007,18 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -1035,7 +1032,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1045,11 +1042,11 @@
       <c r="C2">
         <v>3000</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1059,11 +1056,11 @@
       <c r="C3">
         <v>2000</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1073,11 +1070,11 @@
       <c r="C4">
         <v>4000</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1091,7 +1088,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1105,7 +1102,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1128,66 +1125,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9257DF-418B-48B7-8133-ABF04E7715B5}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:A1048576"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="31.2" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="8"/>
-    <col min="2" max="2" width="148" style="9" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="7"/>
+    <col min="2" max="2" width="148" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="63" x14ac:dyDescent="0.5">
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="B1" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="63" x14ac:dyDescent="0.5">
-      <c r="A2" s="8">
+    <row r="2" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="63" x14ac:dyDescent="0.5">
-      <c r="A3" s="8">
+    <row r="3" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="157.5" x14ac:dyDescent="0.5">
-      <c r="A4" s="8">
+    <row r="4" spans="1:2" ht="156" x14ac:dyDescent="0.6">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="94.5" x14ac:dyDescent="0.5">
-      <c r="A6" s="8">
+    <row r="6" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="A6" s="7">
         <v>4</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="63" x14ac:dyDescent="0.5">
-      <c r="A7" s="8">
+    <row r="7" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="A7" s="7">
         <v>5</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="63" x14ac:dyDescent="0.5">
-      <c r="A9" s="8">
-        <v>6</v>
-      </c>
-      <c r="B9" s="9" t="s">
+    <row r="9" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="A9" s="7">
+        <v>6</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1200,19 +1197,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0262868-F1D2-4471-83DF-330B743CAC3B}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -1226,7 +1223,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1236,11 +1233,11 @@
       <c r="C2">
         <v>1500</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1250,11 +1247,11 @@
       <c r="C3">
         <v>1250</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1264,11 +1261,11 @@
       <c r="C4">
         <v>1000</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1282,7 +1279,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1296,7 +1293,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1310,7 +1307,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1324,7 +1321,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1338,7 +1335,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1352,7 +1349,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1366,7 +1363,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1380,7 +1377,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1394,7 +1391,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1408,7 +1405,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1422,7 +1419,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1436,7 +1433,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1450,7 +1447,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1464,7 +1461,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1478,7 +1475,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -1492,7 +1489,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -1506,7 +1503,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -1520,7 +1517,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -1534,7 +1531,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -1548,7 +1545,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -1562,7 +1559,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1576,7 +1573,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1590,7 +1587,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1610,6 +1607,61 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
+    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j747ac98061d40f0aa7bd47e1db5675d>
+    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <Records_x0020_Date xmlns="ca243fbf-11ff-4731-ae3b-9fc118f3bbf4" xsi:nil="true"/>
+    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
+    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <Records_x0020_Status xmlns="ca243fbf-11ff-4731-ae3b-9fc118f3bbf4">Pending</Records_x0020_Status>
+    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2020-06-12T12:44:56+00:00</Document_x0020_Creation_x0020_Date>
+    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
+    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Creator>
+    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </EPA_x0020_Contributor>
+    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA3E377063FFE5489A04E78E6AF321F7" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0d56b0910c09b2f28088e837fc8a4b1f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xmlns:ns4="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns5="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns6="ca243fbf-11ff-4731-ae3b-9fc118f3bbf4" xmlns:ns7="d75150bc-12f9-4c92-a7eb-e71bcd8ee9be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c38d2d5698dbedce593845e142ad0a0f" ns1:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="" ns7:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2066,62 +2118,44 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5D2AB43-1478-4761-B6C2-35F0AE76DC6E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="d75150bc-12f9-4c92-a7eb-e71bcd8ee9be"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="ca243fbf-11ff-4731-ae3b-9fc118f3bbf4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E301F64B-2E68-42FE-B72F-07064BA5C6EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
-    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j747ac98061d40f0aa7bd47e1db5675d>
-    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <Records_x0020_Date xmlns="ca243fbf-11ff-4731-ae3b-9fc118f3bbf4" xsi:nil="true"/>
-    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
-    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <Records_x0020_Status xmlns="ca243fbf-11ff-4731-ae3b-9fc118f3bbf4">Pending</Records_x0020_Status>
-    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2020-06-12T12:44:56+00:00</Document_x0020_Creation_x0020_Date>
-    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
-    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Creator>
-    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </EPA_x0020_Contributor>
-    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BB79E98-5AD2-42D4-8617-624CBCC2A96C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D265CA-67CD-4AD3-99A3-30810910E78A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2142,41 +2176,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BB79E98-5AD2-42D4-8617-624CBCC2A96C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E301F64B-2E68-42FE-B72F-07064BA5C6EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5D2AB43-1478-4761-B6C2-35F0AE76DC6E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="d75150bc-12f9-4c92-a7eb-e71bcd8ee9be"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="ca243fbf-11ff-4731-ae3b-9fc118f3bbf4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Copy code from USEPA again
Comment my code and paste the code from the PSDM USEPA GitHub again to solve the issue with the empty graph, it is solved this way.
</commit_message>
<xml_diff>
--- a/1Water_treatment_model_USEPA/PSDM/Example_TCE.xlsx
+++ b/1Water_treatment_model_USEPA/PSDM/Example_TCE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathieu\PycharmProjects\Thesis-Activated-Carbon-Modelling\1Water_treatment_model_USEPA\PSDM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA1F490-3FE3-4546-BB5F-2E7CFC9FA6AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4774C161-6A4C-49BD-A4E7-65BC8D30C74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{317BF3F6-A68C-4964-9BC3-AEDC7E3058F4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{317BF3F6-A68C-4964-9BC3-AEDC7E3058F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Properties" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -274,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -297,6 +302,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -315,9 +322,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -355,7 +362,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -461,7 +468,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -603,7 +610,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -685,7 +692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB297697-1B90-46DD-B82E-FCE20BA48421}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -746,7 +753,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -915,15 +922,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401BCFB4-DB77-4CE9-BB3A-E676947AF423}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" zoomScale="145" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -934,7 +941,7 @@
       <c r="B1" t="s">
         <v>36</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="10" t="s">
         <v>41</v>
       </c>
       <c r="D1" t="s">
@@ -948,10 +955,10 @@
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="11">
         <v>50000</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -962,7 +969,7 @@
       <c r="B3">
         <v>174</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="11">
         <v>50000</v>
       </c>
       <c r="D3" t="s">
@@ -976,7 +983,7 @@
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="10">
         <v>0</v>
       </c>
       <c r="D4" t="s">
@@ -990,7 +997,7 @@
       <c r="B5">
         <v>174</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="10">
         <v>0</v>
       </c>
       <c r="D5" t="s">

</xml_diff>